<commit_message>
BalaRaju -Added some files
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -105,13 +105,61 @@
       <c r="A2" s="0"/>
       <c r="B2" s="0" t="inlineStr">
         <is>
+          <t>Vidya Sagar  Pogiri</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>26454.6</v>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
           <t>Balaraju vankala</t>
         </is>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>7420.35</v>
+      <c r="C3" s="0" t="n">
+        <v>35856.5</v>
       </c>
-      <c r="D2" s="0" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Priyanka Muddana</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>49460.8</v>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>pattabhi ramarao</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8701.46</v>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
BalaRaju - Completed TDS
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -109,7 +109,7 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>26454.6</v>
+        <v>27474.7</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -125,7 +125,7 @@
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>35856.5</v>
+        <v>40804.2</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
@@ -141,7 +141,7 @@
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>49460.8</v>
+        <v>58681.4</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
BalaRaju - Added code for organizations
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -105,61 +105,13 @@
       <c r="A2" s="0"/>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Vidya Sagar  Pogiri</t>
+          <t>Balaraju vankala</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>27474.7</v>
+        <v>31780.8</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Balaraju vankala</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>40804.2</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Priyanka Muddana</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>58681.4</v>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>pattabhi ramarao</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>8701.46</v>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
BalaRaju -added code for departments
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -75,7 +75,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
   </cols>
   <sheetData>
@@ -109,7 +109,7 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>7251220.0</v>
+        <v>8333.97</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
sekhar - added changes to leaves
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
@@ -102,16 +102,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
+      <c r="A2" s="0" t="n">
+        <v>32145698741</v>
+      </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Balaraju vankala</t>
+          <t>Priyanka Muddana</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>31780.8</v>
+        <v>9278.96</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>123654789963</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Vidya Sagar pogiri</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9793.33</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
BalaRaju - Completed PayRoll Module
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,15 +67,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
   </cols>
   <sheetData>
@@ -102,36 +102,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>32145698741</v>
-      </c>
+      <c r="A2" s="0"/>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Priyanka Muddana</t>
+          <t>fgfg fgfgfg</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>9278.96</v>
+        <v>0.86</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>123654789963</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Vidya Sagar pogiri</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>9793.33</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
Priyanka my slips modified
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
@@ -102,8 +102,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>32145698741</v>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>7364hlfw89t6</t>
+        </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -111,27 +113,9 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>9278.96</v>
+        <v>1450.25</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>123654789963</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Vidya Sagar pogiri</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>9793.33</v>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
sagar - pay roll modified
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -75,7 +75,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
   </cols>
   <sheetData>
@@ -102,14 +102,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
+      <c r="A2" s="0" t="n">
+        <v>746465465</v>
+      </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>fgfg fgfgfg</t>
+          <t>Vidya Sagar  Pogiri</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.86</v>
+        <v>5291.4</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
changes made to views
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
@@ -102,10 +102,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>7364hlfw89t6</t>
-        </is>
+      <c r="A2" s="0" t="n">
+        <v>32145698741</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -113,9 +111,27 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1450.25</v>
+        <v>40989.1</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>123654789963</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Vidya Sagar pogiri</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9793.33</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>

<commit_message>
Priyanka conflicts resolved with leave history
</commit_message>
<xml_diff>
--- a/public/November-2014-bank_statement.xlsx
+++ b/public/November-2014-bank_statement.xlsx
@@ -67,13 +67,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
@@ -102,10 +102,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>7364hlfw89t6</t>
-        </is>
+      <c r="A2" s="0" t="n">
+        <v>32145698741</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -113,9 +111,27 @@
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1450.25</v>
+        <v>40989.1</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>123654789963</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Vidya Sagar pogiri</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>9793.33</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>November</t>
         </is>

</xml_diff>